<commit_message>
update doc + started implementation granier1999 for transpiration
</commit_message>
<xml_diff>
--- a/documentation/meteorological_input.xlsx
+++ b/documentation/meteorological_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruffault/Dropbox/Mon Mac (MacBook-Pro-de-Julien.local)/Desktop/SurEau-Ecos_V4.0/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146CAC0D-F78E-4140-846D-2D92BB134F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20577CC8-864E-2F41-9E43-9C61CDB21E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4840" yWindow="5340" windowWidth="26840" windowHeight="15940" xr2:uid="{E9C28B1F-0E9B-D14B-B8C2-4A9CDC373CB2}"/>
   </bookViews>
@@ -291,7 +291,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,6 +352,11 @@
       <color theme="1"/>
       <name val="Courrier new"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courrier new"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -382,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -394,6 +399,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +718,7 @@
   <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -745,7 +752,7 @@
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -762,7 +769,7 @@
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -777,7 +784,7 @@
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -792,7 +799,7 @@
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -807,7 +814,7 @@
       <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -822,7 +829,7 @@
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -837,7 +844,7 @@
       <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -852,7 +859,7 @@
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -867,7 +874,7 @@
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -882,7 +889,7 @@
       <c r="C11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="12" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="10" t="s">

</xml_diff>